<commit_message>
remove data, output, and images from version control
</commit_message>
<xml_diff>
--- a/Data/2020_09_08_Bohannan_16S-v4_pmoA_primers.xlsx
+++ b/Data/2020_09_08_Bohannan_16S-v4_pmoA_primers.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet4_2" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="187">
   <si>
     <t xml:space="preserve">IDT Plate Well </t>
   </si>
@@ -491,6 +494,9 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">Remaining F primer</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
@@ -510,17 +516,148 @@
   </si>
   <si>
     <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remaining R primer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Primer set Conc (uM)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Vol (uL)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Primer Set Diluted Conc (uM)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction Vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template Vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Mix Vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other primer vol (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction Conc (uM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final uL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer Vol uL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer conc uM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primer uM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primer uL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final uM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer Dilution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction Setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Mix (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template (uL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remaining (uL)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -558,8 +695,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +745,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -689,7 +840,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,6 +937,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,8 +1057,8 @@
   </sheetPr>
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1407,6 +1598,16 @@
         <f aca="false">I21/M21</f>
         <v>19</v>
       </c>
+      <c r="R21" s="1" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="T21" s="1" t="n">
+        <f aca="false">(P21*R21)/S21</f>
+        <v>0.504385964912281</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
@@ -2413,604 +2614,1816 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="6" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.44"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <f aca="false">SUM(F1:F3)</f>
+        <v>12</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P6" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" s="24" customFormat="true" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D7" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">57 - SUM(F9:Q9)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">57 - SUM(F10:Q10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">57 - SUM(F11:Q11)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">57 - SUM(F12:Q12)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">57 - SUM(F13:Q13)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">57 - SUM(F14:Q14)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">57 - SUM(F9:F14)</f>
+        <v>21</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">57 - SUM(G9:G14)</f>
+        <v>21</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">57 - SUM(H9:H14)</f>
+        <v>21</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">57 - SUM(I9:I14)</f>
+        <v>21</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">57 - SUM(J9:J14)</f>
+        <v>21</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">57 - SUM(K9:K14)</f>
+        <v>39</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">57 - SUM(L9:L14)</f>
+        <v>39</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">57 - SUM(M9:M14)</f>
+        <v>39</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">57 - SUM(N9:N14)</f>
+        <v>39</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">57 - SUM(O9:O14)</f>
+        <v>39</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">57 - SUM(P9:P14)</f>
+        <v>39</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">57 - SUM(Q9:Q14)</f>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="5" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="28" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>149</v>
+    <row r="1" s="26" customFormat="true" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>149</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">(H2*I2)/J2</f>
+        <v>6.57894736842105</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <f aca="false">(L2*M2)/K2</f>
+        <v>1.9</v>
+      </c>
+      <c r="Q2" s="28" t="n">
+        <f aca="false">M2-SUM(N2:P2)</f>
+        <v>5.6</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <f aca="false">(P2*K2)/SUM(N2:Q2)</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>149</v>
+      <c r="A3" s="1"/>
+      <c r="B3" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">(H3*I3)/J3</f>
+        <v>2.19298245614035</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">(L3*M3)/K3</f>
+        <v>5.7</v>
+      </c>
+      <c r="Q3" s="28" t="n">
+        <f aca="false">M3-SUM(N3:P3)</f>
+        <v>1.8</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">(P3*K3)/SUM(N3:P3)</f>
+        <v>0.538793103448276</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="0" t="n">
-        <f aca="false">SUM(E1:E3)</f>
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="A4" s="1"/>
+      <c r="B4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>3</v>
+      <c r="K4" s="0" t="n">
+        <f aca="false">(H4*I4)/J4</f>
+        <v>2.19298245614035</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <f aca="false">(L4*M4)/K4</f>
+        <v>5.7</v>
+      </c>
+      <c r="Q4" s="28" t="n">
+        <f aca="false">M4-SUM(N4:P4)</f>
+        <v>1.8</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <f aca="false">(P4*K4)/SUM(N4:P4)</f>
+        <v>0.538793103448276</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>5</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>4</v>
+        <v>4.3859649122807</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J5" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>7</v>
+        <f aca="false">(H5*I5)/J5</f>
+        <v>4.3859649122807</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>9</v>
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="0" t="s">
+        <f aca="false">(L5*M5)/K5</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q5" s="28" t="n">
+        <f aca="false">M5-SUM(N5:P5)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">(P5*K5)/SUM(N5:P5)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(H6*I6)/J6</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <f aca="false">(L6*M6)/K6</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q6" s="28" t="n">
+        <f aca="false">M6-SUM(N6:P6)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <f aca="false">(P6*K6)/SUM(N6:P6)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">(H7*I7)/J7</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <f aca="false">(L7*M7)/K7</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q7" s="28" t="n">
+        <f aca="false">M7-SUM(N7:P7)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <f aca="false">(P7*K7)/SUM(N7:P7)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">(H8*I8)/J8</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <f aca="false">(L8*M8)/K8</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q8" s="28" t="n">
+        <f aca="false">M8-SUM(N8:P8)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">(P8*K8)/SUM(N8:P8)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="C9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">(H9*I9)/J9</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">(L9*M9)/K9</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q9" s="28" t="n">
+        <f aca="false">M9-SUM(N9:P9)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">(P9*K9)/SUM(N9:P9)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="C10" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">(H10*I10)/J10</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">(L10*M10)/K10</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q10" s="28" t="n">
+        <f aca="false">M10-SUM(N10:P10)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">(P10*K10)/SUM(N10:P10)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="C11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">(H11*I11)/J11</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false">(L11*M11)/K11</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q11" s="28" t="n">
+        <f aca="false">M11-SUM(N11:P11)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">(P11*K11)/SUM(N11:P11)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="C12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">(H12*I12)/J12</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <f aca="false">(L12*M12)/K12</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q12" s="28" t="n">
+        <f aca="false">M12-SUM(N12:P12)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">(P12*K12)/SUM(N12:P12)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="C13" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">(H13*I13)/J13</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <f aca="false">(L13*M13)/K13</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q13" s="28" t="n">
+        <f aca="false">M13-SUM(N13:P13)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">(P13*K13)/SUM(N13:P13)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="C14" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">(H14*I14)/J14</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">(L14*M14)/K14</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q14" s="28" t="n">
+        <f aca="false">M14-SUM(N14:P14)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">(P14*K14)/SUM(N14:P14)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="C15" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">(H15*I15)/J15</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">(L15*M15)/K15</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q15" s="28" t="n">
+        <f aca="false">M15-SUM(N15:P15)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">(P15*K15)/SUM(N15:P15)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="C16" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">(H16*I16)/J16</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">(L16*M16)/K16</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q16" s="28" t="n">
+        <f aca="false">M16-SUM(N16:P16)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">(P16*K16)/SUM(N16:P16)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="C17" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">(H17*I17)/J17</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">(L17*M17)/K17</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q17" s="28" t="n">
+        <f aca="false">M17-SUM(N17:P17)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">(P17*K17)/SUM(N17:P17)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="C18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">(H18*I18)/J18</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P18" s="0" t="n">
+        <f aca="false">(L18*M18)/K18</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q18" s="28" t="n">
+        <f aca="false">M18-SUM(N18:P18)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <f aca="false">(P18*K18)/SUM(N18:P18)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="P6" s="0" t="s">
+      <c r="C19" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">(H19*I19)/J19</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <f aca="false">(L19*M19)/K19</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q19" s="28" t="n">
+        <f aca="false">M19-SUM(N19:P19)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <f aca="false">(P19*K19)/SUM(N19:P19)</f>
+        <v>0.614250614250614</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="23" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="P7" s="0" t="s">
+      <c r="C20" s="18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="P8" s="0" t="s">
+      <c r="D20" s="21" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <f aca="false">57 - SUM(E9:P9)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="0" t="n">
-        <f aca="false">57 - SUM(E10:P10)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="0" t="n">
-        <f aca="false">57 - SUM(E11:P11)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <f aca="false">57 - SUM(E12:P12)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <f aca="false">57 - SUM(E13:P13)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="0" t="n">
-        <f aca="false">57 - SUM(E14:P14)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="30.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <f aca="false">57 - SUM(E9:E14)</f>
-        <v>21</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <f aca="false">57 - SUM(F9:F14)</f>
-        <v>21</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">57 - SUM(G9:G14)</f>
-        <v>21</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">57 - SUM(H9:H14)</f>
-        <v>21</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <f aca="false">57 - SUM(I9:I14)</f>
-        <v>21</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">57 - SUM(J9:J14)</f>
-        <v>39</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">57 - SUM(K9:K14)</f>
-        <v>39</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">57 - SUM(L9:L14)</f>
-        <v>39</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <f aca="false">57 - SUM(M9:M14)</f>
-        <v>39</v>
-      </c>
-      <c r="N15" s="0" t="n">
-        <f aca="false">57 - SUM(N9:N14)</f>
-        <v>39</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <f aca="false">57 - SUM(O9:O14)</f>
-        <v>39</v>
-      </c>
-      <c r="P15" s="0" t="n">
-        <f aca="false">57 - SUM(P9:P14)</f>
-        <v>39</v>
+      <c r="E20" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">(H20*I20)/J20</f>
+        <v>4.3859649122807</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">12.5+11.5+1</f>
+        <v>25</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <f aca="false">(L20*M20)/K20</f>
+        <v>2.85</v>
+      </c>
+      <c r="Q20" s="28" t="n">
+        <f aca="false">M20-SUM(N20:P20)</f>
+        <v>4.65</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <f aca="false">(P20*K20)/SUM(N20:P20)</f>
+        <v>0.614250614250614</v>
       </c>
     </row>
   </sheetData>
@@ -3022,4 +4435,1204 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="26" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="J2" s="30" t="n">
+        <f aca="false">(F2*H2)/I2</f>
+        <v>8</v>
+      </c>
+      <c r="K2" s="30" t="n">
+        <f aca="false">H2</f>
+        <v>2</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">J2-H2-K2</f>
+        <v>4</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <f aca="false">(I2*N2)/M2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G4" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G15" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F16" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G16" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F17" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">(B26*C26)/D26</f>
+        <v>25</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">(B30*C30)/D30</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <f aca="false">(C32*D32)/B32</f>
+        <v>12.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="26" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G3" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">12.5/Q3</f>
+        <v>2.19298245614035</v>
+      </c>
+      <c r="J3" s="30" t="n">
+        <f aca="false">(F3*H3)/I3</f>
+        <v>6</v>
+      </c>
+      <c r="K3" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">J3-H3-K3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="N3" s="32" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="O3" s="32" t="n">
+        <v>5</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <f aca="false">M3-N3-O3</f>
+        <v>7.5</v>
+      </c>
+      <c r="Q3" s="32" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <f aca="false">(I3*Q3)/M3</f>
+        <v>0.5</v>
+      </c>
+      <c r="S3" s="32" t="n">
+        <f aca="false">M3-N3-O3-Q3</f>
+        <v>1.8</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <f aca="false">SUM(S3,Q3,O3,N3)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G4" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G8" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G15" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G16" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>4.3859649122807</v>
+      </c>
+      <c r="G21" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">(B27*C27)/D27</f>
+        <v>25</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <f aca="false">(B31*C31)/D31</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <f aca="false">(C33*D33)/B33</f>
+        <v>12.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:S1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>